<commit_message>
updating currentstatus spread sheet
</commit_message>
<xml_diff>
--- a/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
+++ b/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\dev_space\ttte\projects\The-LeetCode-Engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6275DE2E-85F5-4B4B-B2C2-AF17CAC3C9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E9C417-9C54-4DA2-AEAA-A44759B83332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8390ECE7-BBE1-4ED1-BF24-889CE5C14879}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="155">
   <si>
     <t>Two Sum</t>
   </si>
@@ -284,6 +284,225 @@
   </si>
   <si>
     <t>Min Stack</t>
+  </si>
+  <si>
+    <t>Find Median from Data Stream</t>
+  </si>
+  <si>
+    <t>Serialize and Deserialize Binary Tree</t>
+  </si>
+  <si>
+    <t>Design Tic-Tac-Toe</t>
+  </si>
+  <si>
+    <t>Design Search Auto-Complete System</t>
+  </si>
+  <si>
+    <t>Maximum Frequency Stack</t>
+  </si>
+  <si>
+    <t>Reverse Integer</t>
+  </si>
+  <si>
+    <t>Second Highest Salary</t>
+  </si>
+  <si>
+    <t>Partition Labels</t>
+  </si>
+  <si>
+    <t>Prison Cells after N Days</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Arrays, Strings</t>
+  </si>
+  <si>
+    <t>Linked Lists</t>
+  </si>
+  <si>
+    <t>Trees &amp; Graphs</t>
+  </si>
+  <si>
+    <t>Recursion</t>
+  </si>
+  <si>
+    <t>Sorting &amp; Search</t>
+  </si>
+  <si>
+    <t>Dynamic Prog</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Spiral Matrix II</t>
+  </si>
+  <si>
+    <t>Set Matrix Zeroes</t>
+  </si>
+  <si>
+    <t>Sparse Matrix Multiplication</t>
+  </si>
+  <si>
+    <t>Sort the Matrix Diagonally</t>
+  </si>
+  <si>
+    <t>Sum in a Matrix</t>
+  </si>
+  <si>
+    <t>Search a 2D Matrix II</t>
+  </si>
+  <si>
+    <t>Matrix Cells in Distance Order</t>
+  </si>
+  <si>
+    <t>Shortest path in Binary Matrix</t>
+  </si>
+  <si>
+    <t>Rank transform of a Matrix</t>
+  </si>
+  <si>
+    <t>Lucky numbers in a Matrix</t>
+  </si>
+  <si>
+    <t>Check if Matrix is X-Matrix</t>
+  </si>
+  <si>
+    <t>Build a Matrix with Conditions</t>
+  </si>
+  <si>
+    <t>Array of Objects to Matrix</t>
+  </si>
+  <si>
+    <t>Sum of Matrix after Queries</t>
+  </si>
+  <si>
+    <t>Matrix Similiarity with Cycle Shift</t>
+  </si>
+  <si>
+    <t>Match Alpha-Numeric Pattern in Matrix  I</t>
+  </si>
+  <si>
+    <t>Longest increasing path in a Matrix</t>
+  </si>
+  <si>
+    <t>Reconstruct a 2-Row Binary Matrix</t>
+  </si>
+  <si>
+    <t>Special Positions in a Binary Matrix</t>
+  </si>
+  <si>
+    <t>Largest Local Values in a Matrix</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element in a Sorted Stack</t>
+  </si>
+  <si>
+    <t>Longest Line of Consecutive One in a Matrix</t>
+  </si>
+  <si>
+    <t>Cells with odd values in a Matrix</t>
+  </si>
+  <si>
+    <t>The K Weakest Rows in a Matrix</t>
+  </si>
+  <si>
+    <t>Count negative numbers in a Matrix</t>
+  </si>
+  <si>
+    <t>Maximum non-negative product in a Matrix</t>
+  </si>
+  <si>
+    <t>Median of a Row-wise sorted Matrix</t>
+  </si>
+  <si>
+    <t>Maximum Strictly Increasing cells in a Matrix</t>
+  </si>
+  <si>
+    <t>Find a good subset of the Matrix</t>
+  </si>
+  <si>
+    <t>Find valid matrix given row and column sums</t>
+  </si>
+  <si>
+    <t>Determine weather Matrix can be obtained by rotation</t>
+  </si>
+  <si>
+    <t>Minimum operations to remove adjacent ones in Matrix</t>
+  </si>
+  <si>
+    <t>Minimum number of Flips to convert Binary Matrix to Zero Matrix</t>
+  </si>
+  <si>
+    <t>Paths in Matrix whos sum is divisible by K</t>
+  </si>
+  <si>
+    <t>Find the Kth smallest sum of a Matrix with Sorted Rows</t>
+  </si>
+  <si>
+    <t>Disconnect path in a Binary Matrix by at most one Flip</t>
+  </si>
+  <si>
+    <t>Wildcard Matching</t>
+  </si>
+  <si>
+    <t>Camelcase Matching</t>
+  </si>
+  <si>
+    <t>Regular Expression Matching</t>
+  </si>
+  <si>
+    <t>Matchsticks to Square</t>
+  </si>
+  <si>
+    <t>Output contest matches</t>
+  </si>
+  <si>
+    <t>Repeated String Match</t>
+  </si>
+  <si>
+    <t>DI String Match</t>
+  </si>
+  <si>
+    <t>Number of Matching Sub-Sequences</t>
+  </si>
+  <si>
+    <t>Match substring after replacement</t>
+  </si>
+  <si>
+    <t>String matching in an array</t>
+  </si>
+  <si>
+    <t>Count of matches in Tournament</t>
+  </si>
+  <si>
+    <t>Count items matching a rule</t>
+  </si>
+  <si>
+    <t>All the matches of the league</t>
+  </si>
+  <si>
+    <t>Maximum matching of players with Trainers</t>
+  </si>
+  <si>
+    <t>Flip Binary Tree to Match pre-order traversal</t>
+  </si>
+  <si>
+    <t>The score of students solving math expression</t>
+  </si>
+  <si>
+    <t>Numbers of Subarrays that match a pattern I</t>
+  </si>
+  <si>
+    <t>Number of subarrays that match a pattern II</t>
+  </si>
+  <si>
+    <t>Meta</t>
   </si>
 </sst>
 </file>
@@ -340,7 +559,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -349,6 +568,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,28 +905,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90268034-E08E-4976-8F3C-A958CE4EFA52}">
   <dimension ref="A4:E146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="133" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D119" sqref="D119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>63</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -720,6 +941,12 @@
       <c r="B5" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>44</v>
       </c>
@@ -731,6 +958,12 @@
       <c r="B6" s="1" t="s">
         <v>38</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>44</v>
       </c>
@@ -742,6 +975,12 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>44</v>
       </c>
@@ -753,6 +992,12 @@
       <c r="B8" s="1" t="s">
         <v>67</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>44</v>
       </c>
@@ -764,6 +1009,12 @@
       <c r="B9" s="1" t="s">
         <v>75</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>44</v>
       </c>
@@ -772,7 +1023,15 @@
       <c r="A10" s="1">
         <v>7</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
@@ -784,6 +1043,12 @@
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>44</v>
       </c>
@@ -792,7 +1057,12 @@
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>44</v>
       </c>
@@ -804,6 +1074,12 @@
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C13" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>44</v>
       </c>
@@ -815,6 +1091,12 @@
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>44</v>
       </c>
@@ -826,6 +1108,12 @@
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>44</v>
       </c>
@@ -837,6 +1125,12 @@
       <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C16" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>44</v>
       </c>
@@ -848,6 +1142,12 @@
       <c r="B17" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>44</v>
       </c>
@@ -859,6 +1159,12 @@
       <c r="B18" s="1" t="s">
         <v>61</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>44</v>
       </c>
@@ -870,6 +1176,12 @@
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>44</v>
       </c>
@@ -881,6 +1193,12 @@
       <c r="B20" s="1" t="s">
         <v>64</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>44</v>
       </c>
@@ -892,6 +1210,12 @@
       <c r="B21" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>44</v>
       </c>
@@ -903,6 +1227,12 @@
       <c r="B22" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>44</v>
       </c>
@@ -914,6 +1244,12 @@
       <c r="B23" s="1" t="s">
         <v>68</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>44</v>
       </c>
@@ -925,6 +1261,12 @@
       <c r="B24" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="C24" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>44</v>
       </c>
@@ -933,7 +1275,12 @@
       <c r="A25" s="1">
         <v>44</v>
       </c>
-      <c r="B25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>44</v>
       </c>
@@ -945,6 +1292,12 @@
       <c r="B26" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="C26" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
@@ -956,6 +1309,12 @@
       <c r="B27" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>44</v>
       </c>
@@ -967,6 +1326,12 @@
       <c r="B28" s="1" t="s">
         <v>76</v>
       </c>
+      <c r="C28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>44</v>
       </c>
@@ -978,6 +1343,9 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="D29" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>44</v>
       </c>
@@ -989,6 +1357,12 @@
       <c r="B30" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>44</v>
       </c>
@@ -997,7 +1371,12 @@
       <c r="A31" s="1">
         <v>59</v>
       </c>
-      <c r="B31" s="1"/>
+      <c r="B31" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>44</v>
       </c>
@@ -1006,7 +1385,12 @@
       <c r="A32" s="1">
         <v>73</v>
       </c>
-      <c r="B32" s="1"/>
+      <c r="B32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>44</v>
       </c>
@@ -1018,6 +1402,9 @@
       <c r="B33" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="D33" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>44</v>
       </c>
@@ -1029,6 +1416,12 @@
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>44</v>
       </c>
@@ -1040,6 +1433,12 @@
       <c r="B35" s="1" t="s">
         <v>65</v>
       </c>
+      <c r="C35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>44</v>
       </c>
@@ -1051,6 +1450,12 @@
       <c r="B36" s="1" t="s">
         <v>48</v>
       </c>
+      <c r="C36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>44</v>
       </c>
@@ -1062,6 +1467,12 @@
       <c r="B37" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="C37" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>44</v>
       </c>
@@ -1073,6 +1484,12 @@
       <c r="B38" s="1" t="s">
         <v>50</v>
       </c>
+      <c r="C38" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>44</v>
       </c>
@@ -1084,6 +1501,12 @@
       <c r="B39" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="C39" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>44</v>
       </c>
@@ -1093,6 +1516,9 @@
         <v>104</v>
       </c>
       <c r="B40" s="1"/>
+      <c r="D40" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>44</v>
       </c>
@@ -1102,6 +1528,9 @@
         <v>105</v>
       </c>
       <c r="B41" s="1"/>
+      <c r="D41" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>44</v>
       </c>
@@ -1111,6 +1540,9 @@
         <v>106</v>
       </c>
       <c r="B42" s="1"/>
+      <c r="D42" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E42" s="1" t="s">
         <v>44</v>
       </c>
@@ -1122,6 +1554,12 @@
       <c r="B43" s="1" t="s">
         <v>77</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>44</v>
       </c>
@@ -1133,6 +1571,12 @@
       <c r="B44" s="1" t="s">
         <v>52</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>44</v>
       </c>
@@ -1144,6 +1588,12 @@
       <c r="B45" s="1" t="s">
         <v>53</v>
       </c>
+      <c r="C45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>44</v>
       </c>
@@ -1155,6 +1605,12 @@
       <c r="B46" s="1" t="s">
         <v>54</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>44</v>
       </c>
@@ -1166,6 +1622,12 @@
       <c r="B47" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="C47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>44</v>
       </c>
@@ -1177,6 +1639,12 @@
       <c r="B48" s="1" t="s">
         <v>78</v>
       </c>
+      <c r="C48" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>44</v>
       </c>
@@ -1188,6 +1656,12 @@
       <c r="B49" s="1" t="s">
         <v>80</v>
       </c>
+      <c r="C49" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>44</v>
       </c>
@@ -1199,6 +1673,12 @@
       <c r="B50" s="1" t="s">
         <v>81</v>
       </c>
+      <c r="C50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>44</v>
       </c>
@@ -1210,6 +1690,12 @@
       <c r="B51" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="C51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>44</v>
       </c>
@@ -1221,6 +1707,12 @@
       <c r="B52" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="C52" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>44</v>
       </c>
@@ -1229,7 +1721,15 @@
       <c r="A53" s="1">
         <v>176</v>
       </c>
-      <c r="B53" s="1"/>
+      <c r="B53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>44</v>
       </c>
@@ -1241,6 +1741,12 @@
       <c r="B54" s="1" t="s">
         <v>55</v>
       </c>
+      <c r="C54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>44</v>
       </c>
@@ -1252,6 +1758,12 @@
       <c r="B55" s="1" t="s">
         <v>46</v>
       </c>
+      <c r="C55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E55" s="1" t="s">
         <v>44</v>
       </c>
@@ -1263,6 +1775,12 @@
       <c r="B56" s="1" t="s">
         <v>56</v>
       </c>
+      <c r="C56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>44</v>
       </c>
@@ -1274,6 +1792,12 @@
       <c r="B57" s="1" t="s">
         <v>66</v>
       </c>
+      <c r="C57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>44</v>
       </c>
@@ -1285,6 +1809,12 @@
       <c r="B58" s="1" t="s">
         <v>71</v>
       </c>
+      <c r="C58" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>44</v>
       </c>
@@ -1296,6 +1826,12 @@
       <c r="B59" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="C59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>44</v>
       </c>
@@ -1307,6 +1843,12 @@
       <c r="B60" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="C60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>44</v>
       </c>
@@ -1315,7 +1857,12 @@
       <c r="A61" s="1">
         <v>240</v>
       </c>
-      <c r="B61" s="1"/>
+      <c r="B61" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>44</v>
       </c>
@@ -1327,6 +1874,12 @@
       <c r="B62" s="1" t="s">
         <v>72</v>
       </c>
+      <c r="C62" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E62" s="1" t="s">
         <v>44</v>
       </c>
@@ -1338,6 +1891,12 @@
       <c r="B63" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="C63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>44</v>
       </c>
@@ -1349,6 +1908,12 @@
       <c r="B64" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>44</v>
       </c>
@@ -1357,7 +1922,15 @@
       <c r="A65" s="1">
         <v>295</v>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>44</v>
       </c>
@@ -1366,7 +1939,15 @@
       <c r="A66" s="1">
         <v>297</v>
       </c>
-      <c r="B66" s="1"/>
+      <c r="B66" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>44</v>
       </c>
@@ -1375,7 +1956,12 @@
       <c r="A67" s="1">
         <v>311</v>
       </c>
-      <c r="B67" s="1"/>
+      <c r="B67" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E67" s="1" t="s">
         <v>44</v>
       </c>
@@ -1387,6 +1973,12 @@
       <c r="B68" s="1" t="s">
         <v>79</v>
       </c>
+      <c r="C68" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>44</v>
       </c>
@@ -1395,7 +1987,12 @@
       <c r="A69" s="1">
         <v>329</v>
       </c>
-      <c r="B69" s="1"/>
+      <c r="B69" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E69" s="1" t="s">
         <v>44</v>
       </c>
@@ -1407,6 +2004,12 @@
       <c r="B70" s="1" t="s">
         <v>73</v>
       </c>
+      <c r="C70" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E70" s="1" t="s">
         <v>44</v>
       </c>
@@ -1415,7 +2018,15 @@
       <c r="A71" s="1">
         <v>348</v>
       </c>
-      <c r="B71" s="1"/>
+      <c r="B71" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E71" s="1" t="s">
         <v>44</v>
       </c>
@@ -1424,7 +2035,12 @@
       <c r="A72" s="1">
         <v>378</v>
       </c>
-      <c r="B72" s="1"/>
+      <c r="B72" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E72" s="1" t="s">
         <v>44</v>
       </c>
@@ -1436,6 +2052,12 @@
       <c r="B73" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="C73" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E73" s="1" t="s">
         <v>44</v>
       </c>
@@ -1444,7 +2066,12 @@
       <c r="A74" s="1">
         <v>473</v>
       </c>
-      <c r="B74" s="1"/>
+      <c r="B74" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>44</v>
       </c>
@@ -1456,6 +2083,9 @@
       <c r="B75" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="D75" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E75" s="1" t="s">
         <v>44</v>
       </c>
@@ -1467,6 +2097,9 @@
       <c r="B76" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="D76" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E76" s="1" t="s">
         <v>44</v>
       </c>
@@ -1478,6 +2111,12 @@
       <c r="B77" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="C77" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E77" s="1" t="s">
         <v>44</v>
       </c>
@@ -1486,7 +2125,12 @@
       <c r="A78" s="1">
         <v>544</v>
       </c>
-      <c r="B78" s="1"/>
+      <c r="B78" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E78" s="1" t="s">
         <v>44</v>
       </c>
@@ -1495,7 +2139,12 @@
       <c r="A79" s="1">
         <v>562</v>
       </c>
-      <c r="B79" s="1"/>
+      <c r="B79" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E79" s="1" t="s">
         <v>44</v>
       </c>
@@ -1507,6 +2156,9 @@
       <c r="B80" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="D80" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E80" s="1" t="s">
         <v>44</v>
       </c>
@@ -1515,7 +2167,15 @@
       <c r="A81" s="1">
         <v>642</v>
       </c>
-      <c r="B81" s="1"/>
+      <c r="B81" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E81" s="1" t="s">
         <v>44</v>
       </c>
@@ -1527,6 +2187,12 @@
       <c r="B82" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="C82" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E82" s="1" t="s">
         <v>44</v>
       </c>
@@ -1538,6 +2204,12 @@
       <c r="B83" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="C83" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E83" s="1" t="s">
         <v>44</v>
       </c>
@@ -1546,7 +2218,12 @@
       <c r="A84" s="1">
         <v>686</v>
       </c>
-      <c r="B84" s="1"/>
+      <c r="B84" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E84" s="1" t="s">
         <v>44</v>
       </c>
@@ -1558,6 +2235,12 @@
       <c r="B85" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="C85" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E85" s="1" t="s">
         <v>44</v>
       </c>
@@ -1569,6 +2252,9 @@
       <c r="B86" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="D86" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E86" s="1" t="s">
         <v>44</v>
       </c>
@@ -1577,7 +2263,15 @@
       <c r="A87" s="1">
         <v>763</v>
       </c>
-      <c r="B87" s="1"/>
+      <c r="B87" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E87" s="1" t="s">
         <v>44</v>
       </c>
@@ -1589,6 +2283,9 @@
       <c r="B88" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="D88" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E88" s="1" t="s">
         <v>44</v>
       </c>
@@ -1597,7 +2294,12 @@
       <c r="A89" s="1">
         <v>792</v>
       </c>
-      <c r="B89" s="1"/>
+      <c r="B89" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E89" s="1" t="s">
         <v>44</v>
       </c>
@@ -1609,6 +2311,12 @@
       <c r="B90" s="1" t="s">
         <v>35</v>
       </c>
+      <c r="C90" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E90" s="1" t="s">
         <v>44</v>
       </c>
@@ -1620,6 +2328,9 @@
       <c r="B91" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="D91" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E91" s="1" t="s">
         <v>44</v>
       </c>
@@ -1631,6 +2342,9 @@
       <c r="B92" s="1" t="s">
         <v>29</v>
       </c>
+      <c r="D92" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E92" s="1" t="s">
         <v>44</v>
       </c>
@@ -1642,6 +2356,9 @@
       <c r="B93" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="D93" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E93" s="1" t="s">
         <v>44</v>
       </c>
@@ -1650,7 +2367,15 @@
       <c r="A94" s="1">
         <v>895</v>
       </c>
-      <c r="B94" s="1"/>
+      <c r="B94" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E94" s="1" t="s">
         <v>44</v>
       </c>
@@ -1662,6 +2387,12 @@
       <c r="B95" s="1" t="s">
         <v>36</v>
       </c>
+      <c r="C95" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E95" s="1" t="s">
         <v>44</v>
       </c>
@@ -1670,7 +2401,12 @@
       <c r="A96" s="1">
         <v>942</v>
       </c>
-      <c r="B96" s="1"/>
+      <c r="B96" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E96" s="1" t="s">
         <v>44</v>
       </c>
@@ -1679,7 +2415,15 @@
       <c r="A97" s="1">
         <v>957</v>
       </c>
-      <c r="B97" s="1"/>
+      <c r="B97" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E97" s="1" t="s">
         <v>44</v>
       </c>
@@ -1688,7 +2432,12 @@
       <c r="A98" s="1">
         <v>971</v>
       </c>
-      <c r="B98" s="1"/>
+      <c r="B98" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E98" s="1" t="s">
         <v>44</v>
       </c>
@@ -1700,6 +2449,12 @@
       <c r="B99" s="1" t="s">
         <v>74</v>
       </c>
+      <c r="C99" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="E99" s="1" t="s">
         <v>44</v>
       </c>
@@ -1708,7 +2463,12 @@
       <c r="A100" s="1">
         <v>1023</v>
       </c>
-      <c r="B100" s="1"/>
+      <c r="B100" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E100" s="1" t="s">
         <v>44</v>
       </c>
@@ -1717,7 +2477,12 @@
       <c r="A101" s="1">
         <v>1030</v>
       </c>
-      <c r="B101" s="1"/>
+      <c r="B101" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E101" s="1" t="s">
         <v>44</v>
       </c>
@@ -1726,7 +2491,12 @@
       <c r="A102" s="1">
         <v>1091</v>
       </c>
-      <c r="B102" s="1"/>
+      <c r="B102" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E102" s="1" t="s">
         <v>44</v>
       </c>
@@ -1738,6 +2508,9 @@
       <c r="B103" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D103" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E103" s="1" t="s">
         <v>44</v>
       </c>
@@ -1746,7 +2519,12 @@
       <c r="A104" s="1">
         <v>1252</v>
       </c>
-      <c r="B104" s="1"/>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E104" s="1" t="s">
         <v>44</v>
       </c>
@@ -1755,7 +2533,12 @@
       <c r="A105" s="1">
         <v>1253</v>
       </c>
-      <c r="B105" s="1"/>
+      <c r="B105" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E105" s="1" t="s">
         <v>44</v>
       </c>
@@ -1764,7 +2547,12 @@
       <c r="A106" s="1">
         <v>1284</v>
       </c>
-      <c r="B106" s="1"/>
+      <c r="B106" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E106" s="1" t="s">
         <v>44</v>
       </c>
@@ -1776,6 +2564,9 @@
       <c r="B107" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="D107" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E107" s="1" t="s">
         <v>44</v>
       </c>
@@ -1784,7 +2575,12 @@
       <c r="A108" s="1">
         <v>1329</v>
       </c>
-      <c r="B108" s="1"/>
+      <c r="B108" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E108" s="1" t="s">
         <v>44</v>
       </c>
@@ -1793,7 +2589,12 @@
       <c r="A109" s="1">
         <v>1337</v>
       </c>
-      <c r="B109" s="1"/>
+      <c r="B109" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E109" s="1" t="s">
         <v>44</v>
       </c>
@@ -1802,7 +2603,12 @@
       <c r="A110" s="1">
         <v>1351</v>
       </c>
-      <c r="B110" s="1"/>
+      <c r="B110" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E110" s="1" t="s">
         <v>44</v>
       </c>
@@ -1811,7 +2617,12 @@
       <c r="A111" s="1">
         <v>1380</v>
       </c>
-      <c r="B111" s="1"/>
+      <c r="B111" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E111" s="1" t="s">
         <v>44</v>
       </c>
@@ -1820,7 +2631,12 @@
       <c r="A112" s="1">
         <v>1408</v>
       </c>
-      <c r="B112" s="1"/>
+      <c r="B112" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E112" s="1" t="s">
         <v>44</v>
       </c>
@@ -1829,7 +2645,12 @@
       <c r="A113" s="1">
         <v>1439</v>
       </c>
-      <c r="B113" s="1"/>
+      <c r="B113" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E113" s="1" t="s">
         <v>44</v>
       </c>
@@ -1841,6 +2662,9 @@
       <c r="B114" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="D114" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E114" s="1" t="s">
         <v>44</v>
       </c>
@@ -1849,7 +2673,12 @@
       <c r="A115" s="1">
         <v>1582</v>
       </c>
-      <c r="B115" s="1"/>
+      <c r="B115" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D115" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E115" s="1" t="s">
         <v>44</v>
       </c>
@@ -1858,7 +2687,12 @@
       <c r="A116" s="1">
         <v>1594</v>
       </c>
-      <c r="B116" s="1"/>
+      <c r="B116" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D116" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E116" s="1" t="s">
         <v>44</v>
       </c>
@@ -1867,7 +2701,12 @@
       <c r="A117" s="1">
         <v>1605</v>
       </c>
-      <c r="B117" s="1"/>
+      <c r="B117" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D117" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E117" s="1" t="s">
         <v>44</v>
       </c>
@@ -1876,7 +2715,12 @@
       <c r="A118" s="1">
         <v>1632</v>
       </c>
-      <c r="B118" s="1"/>
+      <c r="B118" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E118" s="1" t="s">
         <v>44</v>
       </c>
@@ -1885,7 +2729,12 @@
       <c r="A119" s="1">
         <v>1688</v>
       </c>
-      <c r="B119" s="1"/>
+      <c r="B119" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E119" s="1" t="s">
         <v>44</v>
       </c>
@@ -1894,7 +2743,12 @@
       <c r="A120" s="1">
         <v>1773</v>
       </c>
-      <c r="B120" s="1"/>
+      <c r="B120" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D120" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E120" s="1" t="s">
         <v>44</v>
       </c>
@@ -1903,7 +2757,12 @@
       <c r="A121" s="1">
         <v>1886</v>
       </c>
-      <c r="B121" s="1"/>
+      <c r="B121" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D121" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E121" s="1" t="s">
         <v>44</v>
       </c>
@@ -1915,6 +2774,9 @@
       <c r="B122" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="D122" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E122" s="1" t="s">
         <v>44</v>
       </c>
@@ -1923,7 +2785,12 @@
       <c r="A123" s="1">
         <v>2019</v>
       </c>
-      <c r="B123" s="1"/>
+      <c r="B123" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D123" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E123" s="1" t="s">
         <v>44</v>
       </c>
@@ -1932,7 +2799,12 @@
       <c r="A124" s="1">
         <v>2123</v>
       </c>
-      <c r="B124" s="1"/>
+      <c r="B124" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D124" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E124" s="1" t="s">
         <v>44</v>
       </c>
@@ -1941,7 +2813,12 @@
       <c r="A125" s="1">
         <v>2301</v>
       </c>
-      <c r="B125" s="1"/>
+      <c r="B125" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E125" s="1" t="s">
         <v>44</v>
       </c>
@@ -1950,7 +2827,12 @@
       <c r="A126" s="1">
         <v>2319</v>
       </c>
-      <c r="B126" s="1"/>
+      <c r="B126" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D126" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E126" s="1" t="s">
         <v>44</v>
       </c>
@@ -1962,6 +2844,9 @@
       <c r="B127" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="D127" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E127" s="1" t="s">
         <v>44</v>
       </c>
@@ -1970,7 +2855,12 @@
       <c r="A128" s="1">
         <v>2339</v>
       </c>
-      <c r="B128" s="1"/>
+      <c r="B128" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D128" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E128" s="1" t="s">
         <v>44</v>
       </c>
@@ -1979,7 +2869,12 @@
       <c r="A129" s="1">
         <v>2373</v>
       </c>
-      <c r="B129" s="1"/>
+      <c r="B129" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D129" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E129" s="1" t="s">
         <v>44</v>
       </c>
@@ -1988,7 +2883,12 @@
       <c r="A130" s="1">
         <v>2387</v>
       </c>
-      <c r="B130" s="1"/>
+      <c r="B130" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D130" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E130" s="1" t="s">
         <v>44</v>
       </c>
@@ -1997,7 +2897,12 @@
       <c r="A131" s="1">
         <v>2392</v>
       </c>
-      <c r="B131" s="1"/>
+      <c r="B131" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D131" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E131" s="1" t="s">
         <v>44</v>
       </c>
@@ -2006,7 +2911,12 @@
       <c r="A132" s="1">
         <v>2410</v>
       </c>
-      <c r="B132" s="1"/>
+      <c r="B132" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D132" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E132" s="1" t="s">
         <v>44</v>
       </c>
@@ -2015,7 +2925,12 @@
       <c r="A133" s="1">
         <v>2435</v>
       </c>
-      <c r="B133" s="1"/>
+      <c r="B133" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D133" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E133" s="1" t="s">
         <v>44</v>
       </c>
@@ -2024,7 +2939,12 @@
       <c r="A134" s="1">
         <v>2556</v>
       </c>
-      <c r="B134" s="1"/>
+      <c r="B134" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D134" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E134" s="1" t="s">
         <v>44</v>
       </c>
@@ -2033,7 +2953,12 @@
       <c r="A135" s="1">
         <v>2675</v>
       </c>
-      <c r="B135" s="1"/>
+      <c r="B135" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D135" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E135" s="1" t="s">
         <v>44</v>
       </c>
@@ -2042,7 +2967,12 @@
       <c r="A136" s="1">
         <v>2679</v>
       </c>
-      <c r="B136" s="1"/>
+      <c r="B136" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D136" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E136" s="1" t="s">
         <v>44</v>
       </c>
@@ -2051,7 +2981,12 @@
       <c r="A137" s="1">
         <v>2713</v>
       </c>
-      <c r="B137" s="1"/>
+      <c r="B137" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D137" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E137" s="1" t="s">
         <v>44</v>
       </c>
@@ -2060,7 +2995,12 @@
       <c r="A138" s="1">
         <v>2718</v>
       </c>
-      <c r="B138" s="1"/>
+      <c r="B138" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D138" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E138" s="1" t="s">
         <v>44</v>
       </c>
@@ -2069,7 +3009,12 @@
       <c r="A139" s="1">
         <v>2732</v>
       </c>
-      <c r="B139" s="1"/>
+      <c r="B139" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D139" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E139" s="1" t="s">
         <v>44</v>
       </c>
@@ -2081,6 +3026,9 @@
       <c r="B140" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="D140" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E140" s="1" t="s">
         <v>44</v>
       </c>
@@ -2089,7 +3037,12 @@
       <c r="A141" s="1">
         <v>2946</v>
       </c>
-      <c r="B141" s="1"/>
+      <c r="B141" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D141" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E141" s="1" t="s">
         <v>44</v>
       </c>
@@ -2101,6 +3054,9 @@
       <c r="B142" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="D142" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E142" s="1" t="s">
         <v>44</v>
       </c>
@@ -2109,7 +3065,12 @@
       <c r="A143" s="1">
         <v>3034</v>
       </c>
-      <c r="B143" s="1"/>
+      <c r="B143" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D143" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E143" s="1" t="s">
         <v>44</v>
       </c>
@@ -2118,7 +3079,12 @@
       <c r="A144" s="1">
         <v>3036</v>
       </c>
-      <c r="B144" s="1"/>
+      <c r="B144" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D144" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E144" s="1" t="s">
         <v>44</v>
       </c>
@@ -2127,7 +3093,12 @@
       <c r="A145" s="1">
         <v>3078</v>
       </c>
-      <c r="B145" s="1"/>
+      <c r="B145" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D145" s="4" t="s">
+        <v>154</v>
+      </c>
       <c r="E145" s="1" t="s">
         <v>44</v>
       </c>
@@ -2138,6 +3109,9 @@
       </c>
       <c r="B146" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="D146" s="4" t="s">
+        <v>154</v>
       </c>
       <c r="E146" s="1" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
adding updates for BST, Matrix
</commit_message>
<xml_diff>
--- a/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
+++ b/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\dev_space\ttte\projects\The-LeetCode-Engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6B3300-295E-420D-83ED-A574DDC9523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0B5F94-5E62-4691-B3AF-89327ED4BEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8390ECE7-BBE1-4ED1-BF24-889CE5C14879}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="226">
   <si>
     <t>Two Sum</t>
   </si>
@@ -707,6 +707,15 @@
   </si>
   <si>
     <t>Matrices</t>
+  </si>
+  <si>
+    <t>Maximum Depth of a Binary Tree</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Pre-Order and In-order Traversal</t>
+  </si>
+  <si>
+    <t>Construct Binary Tree from Inorder and Post-Order Traversal</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90268034-E08E-4976-8F3C-A958CE4EFA52}">
   <dimension ref="A1:F144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1535,23 +1544,23 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="4">
         <v>25</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E20" s="6" t="s">
+      <c r="D20" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>44</v>
+      <c r="F20" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1653,63 +1662,63 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="4">
         <v>53</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="6" t="s">
+      <c r="D26" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>184</v>
       </c>
-      <c r="F26" s="1" t="s">
-        <v>44</v>
+      <c r="F26" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="4">
         <v>54</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="D27" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E27" s="6" t="s">
+      <c r="D27" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>185</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>44</v>
+      <c r="F27" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="4">
         <v>56</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D28" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E28" s="6" t="s">
+      <c r="D28" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="F28" s="1" t="s">
-        <v>44</v>
+      <c r="F28" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1813,43 +1822,43 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="4">
         <v>98</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D34" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E34" s="6" t="s">
+      <c r="D34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F34" s="1" t="s">
-        <v>44</v>
+      <c r="F34" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="4">
         <v>101</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C35" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D35" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E35" s="6" t="s">
+      <c r="D35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>190</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>44</v>
+      <c r="F35" s="4" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1896,7 +1905,9 @@
       <c r="A38" s="1">
         <v>104</v>
       </c>
-      <c r="B38" s="1"/>
+      <c r="B38" s="1" t="s">
+        <v>223</v>
+      </c>
       <c r="C38" s="1" t="s">
         <v>94</v>
       </c>
@@ -1914,7 +1925,9 @@
       <c r="A39" s="1">
         <v>105</v>
       </c>
-      <c r="B39" s="1"/>
+      <c r="B39" s="1" t="s">
+        <v>224</v>
+      </c>
       <c r="C39" s="1" t="s">
         <v>94</v>
       </c>
@@ -1932,7 +1945,9 @@
       <c r="A40" s="1">
         <v>106</v>
       </c>
-      <c r="B40" s="1"/>
+      <c r="B40" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C40" s="1" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
doing a full commit of all non-committed artifacts for Jordi Chen to review
</commit_message>
<xml_diff>
--- a/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
+++ b/projects/The-LeetCode-Engineer/CurrentStatus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\dev_space\ttte\projects\The-LeetCode-Engineer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1728BA-F3E4-4F30-BAAD-A3A2ABBBDCC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA65B887-481A-4CB2-A349-25124EC5B645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8390ECE7-BBE1-4ED1-BF24-889CE5C14879}"/>
+    <workbookView xWindow="5745" yWindow="2820" windowWidth="21600" windowHeight="11295" xr2:uid="{8390ECE7-BBE1-4ED1-BF24-889CE5C14879}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="273">
   <si>
     <t>Two Sum</t>
   </si>
@@ -736,10 +736,127 @@
     <t>BST</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Same Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-inorder-traversal/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-binary-search-trees-ii/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/unique-binary-search-trees/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/same-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/recover-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-level-order-traversal-ii/</t>
+  </si>
+  <si>
+    <t>Binary Tree Level-Order Traversal II</t>
+  </si>
+  <si>
+    <t>Convert Sorted Array to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-sorted-array-to-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/convert-sorted-list-to-binary-search-tree/</t>
+  </si>
+  <si>
+    <t>Convert Sorted List to Binary Search Tree</t>
+  </si>
+  <si>
+    <t>Balanced Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/balanced-binary-tree/</t>
+  </si>
+  <si>
+    <t>Minimum Depth of Binary Tree</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/minimum-depth-of-binary-tree/</t>
+  </si>
+  <si>
+    <t>Path Sum</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum/</t>
+  </si>
+  <si>
+    <t>Path Sum II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/path-sum-ii/</t>
+  </si>
+  <si>
+    <t>Flatten Binary Tree to Linked List</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/flatten-binary-tree-to-linked-list/</t>
+  </si>
+  <si>
+    <t>Distinct Subsequences</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node</t>
+  </si>
+  <si>
+    <t>Populating Next Right Pointers in Each Node II</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/distinct-subsequences/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/populating-next-right-pointers-in-each-node/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/populating-next-right-pointers-in-each-node-ii/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/add-two-numbers/description/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-preorder-traversal/</t>
+  </si>
+  <si>
+    <t>Binary Tree Pre-Order Traversal</t>
+  </si>
+  <si>
+    <t>Binary Tree Post-Order Traversal</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-postorder-traversal/</t>
+  </si>
+  <si>
+    <t>Binary Tree Upside Down</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-tree-upside-down/</t>
+  </si>
+  <si>
+    <t>Binary Search Tree Iterator</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/binary-search-tree-iterator/</t>
+  </si>
+  <si>
+    <t>Kth Smallest Element in a BST</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/kth-smallest-element-in-a-bst/</t>
+  </si>
+  <si>
+    <t>https://leetcode.com/problems/lowest-common-ancestor-of-a-binary-search-tree/description/</t>
+  </si>
+  <si>
+    <t>Lowest Common Ancestor of Binary Search Tree</t>
   </si>
 </sst>
 </file>
@@ -790,7 +907,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -812,6 +929,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -843,8 +966,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1182,8 +1305,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90268034-E08E-4976-8F3C-A958CE4EFA52}">
   <dimension ref="A1:G199"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D204" sqref="D204"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1251,7 +1374,9 @@
       <c r="D3" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="E3" s="4"/>
+      <c r="E3" s="5" t="s">
+        <v>260</v>
+      </c>
       <c r="F3" s="4" t="s">
         <v>156</v>
       </c>
@@ -1495,20 +1620,20 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="4">
+      <c r="A16" s="9">
         <v>20</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="9" t="s">
         <v>156</v>
       </c>
     </row>
@@ -1851,56 +1976,62 @@
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="4">
         <v>94</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E34" s="6"/>
-      <c r="F34" s="1" t="s">
+      <c r="C34" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="F34" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="9">
         <v>95</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="9" t="s">
         <v>228</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E35" s="6"/>
-      <c r="F35" s="1" t="s">
+      <c r="C35" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="F35" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="9">
         <v>96</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E36" s="6"/>
-      <c r="F36" s="1" t="s">
+      <c r="C36" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>235</v>
+      </c>
+      <c r="F36" s="9" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1925,38 +2056,42 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="9">
         <v>99</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E38" s="1" t="s">
+      <c r="C38" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D38" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>100</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
-        <v>100</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>155</v>
-      </c>
+      <c r="C39" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="F39" s="9"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
@@ -2019,196 +2154,284 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="9">
         <v>104</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="C43" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D43" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="D43" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E43" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="F43" s="9" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="1">
+      <c r="A44" s="9">
         <v>105</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C44" s="1" t="s">
+      <c r="C44" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E44" s="6" t="s">
+      <c r="D44" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E44" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="F44" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1">
+      <c r="A45" s="9">
         <v>106</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C45" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E45" s="6" t="s">
+      <c r="D45" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="F45" s="9" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="9">
         <v>107</v>
       </c>
-      <c r="C46" t="s">
-        <v>231</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E46" s="9"/>
+      <c r="B46" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>238</v>
+      </c>
+      <c r="F46" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="9">
         <v>108</v>
       </c>
-      <c r="C47" t="s">
-        <v>231</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="9"/>
+      <c r="B47" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="F47" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="9">
         <v>109</v>
       </c>
-      <c r="C48" t="s">
-        <v>231</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="9"/>
+      <c r="B48" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E48" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="F48" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="9">
         <v>110</v>
       </c>
-      <c r="C49" t="s">
-        <v>231</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" s="9"/>
+      <c r="B49" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C49" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D49" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="F49" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="9">
         <v>111</v>
       </c>
-      <c r="C50" t="s">
-        <v>231</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E50" s="9"/>
+      <c r="B50" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="F50" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="9">
         <v>112</v>
       </c>
-      <c r="C51" t="s">
-        <v>231</v>
-      </c>
-      <c r="D51" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E51" s="9"/>
+      <c r="B51" s="9" t="s">
+        <v>248</v>
+      </c>
+      <c r="C51" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>249</v>
+      </c>
+      <c r="F51" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="9">
         <v>113</v>
       </c>
-      <c r="C52" t="s">
-        <v>231</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E52" s="9"/>
+      <c r="B52" s="9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C52" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53">
+      <c r="A53" s="9">
         <v>114</v>
       </c>
-      <c r="C53" t="s">
-        <v>231</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E53" s="9"/>
+      <c r="B53" s="9" t="s">
+        <v>252</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="10" t="s">
+        <v>253</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54">
+      <c r="A54" s="9">
         <v>115</v>
       </c>
-      <c r="C54" t="s">
-        <v>231</v>
-      </c>
-      <c r="D54" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E54" s="9"/>
+      <c r="B54" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D54" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F54" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55">
+      <c r="A55" s="9">
         <v>116</v>
       </c>
-      <c r="C55" t="s">
-        <v>231</v>
-      </c>
-      <c r="D55" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E55" s="9"/>
+      <c r="B55" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="C55" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E55" s="10" t="s">
+        <v>258</v>
+      </c>
+      <c r="F55" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56">
+      <c r="A56" s="9">
         <v>117</v>
       </c>
-      <c r="C56" t="s">
-        <v>231</v>
-      </c>
-      <c r="D56" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E56" s="9"/>
+      <c r="B56" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="C56" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E56" s="10" t="s">
+        <v>259</v>
+      </c>
+      <c r="F56" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
@@ -2331,28 +2554,44 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63">
+      <c r="A63" s="9">
         <v>144</v>
       </c>
-      <c r="C63" t="s">
-        <v>231</v>
-      </c>
-      <c r="D63" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E63" s="9"/>
+      <c r="B63" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="C63" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E63" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F63" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64">
+      <c r="A64" s="9">
         <v>145</v>
       </c>
-      <c r="C64" t="s">
-        <v>231</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E64" s="9"/>
+      <c r="B64" s="9" t="s">
+        <v>263</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D64" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E64" s="10" t="s">
+        <v>264</v>
+      </c>
+      <c r="F64" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
@@ -2395,16 +2634,22 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67">
+      <c r="A67" s="9">
         <v>156</v>
       </c>
-      <c r="C67" t="s">
-        <v>231</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E67" s="9"/>
+      <c r="B67" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="C67" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D67" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E67" s="10" t="s">
+        <v>266</v>
+      </c>
+      <c r="F67" s="9"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
@@ -2447,16 +2692,24 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70">
+      <c r="A70" s="9">
         <v>173</v>
       </c>
-      <c r="C70" t="s">
-        <v>231</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E70" s="9"/>
+      <c r="B70" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F70" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
@@ -2579,28 +2832,44 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77">
+      <c r="A77" s="9">
         <v>230</v>
       </c>
-      <c r="C77" t="s">
-        <v>231</v>
-      </c>
-      <c r="D77" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E77" s="9"/>
+      <c r="B77" s="9" t="s">
+        <v>269</v>
+      </c>
+      <c r="C77" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E77" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="F77" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78">
+      <c r="A78" s="9">
         <v>235</v>
       </c>
-      <c r="C78" t="s">
-        <v>231</v>
-      </c>
-      <c r="D78" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E78" s="9"/>
+      <c r="B78" s="9" t="s">
+        <v>272</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="F78" s="9" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
@@ -2683,28 +2952,32 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83">
+      <c r="A83" s="9">
         <v>255</v>
       </c>
-      <c r="C83" t="s">
-        <v>231</v>
-      </c>
-      <c r="D83" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E83" s="9"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E83" s="10"/>
+      <c r="F83" s="9"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84">
+      <c r="A84" s="9">
         <v>257</v>
       </c>
-      <c r="C84" t="s">
-        <v>231</v>
-      </c>
-      <c r="D84" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E84" s="9"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E84" s="10"/>
+      <c r="F84" s="9"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
@@ -2727,28 +3000,32 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86">
+      <c r="A86" s="9">
         <v>270</v>
       </c>
-      <c r="C86" t="s">
-        <v>231</v>
-      </c>
-      <c r="D86" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E86" s="10"/>
+      <c r="F86" s="9"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87">
+      <c r="A87" s="9">
         <v>272</v>
       </c>
-      <c r="C87" t="s">
-        <v>231</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E87" s="9"/>
+      <c r="B87" s="9"/>
+      <c r="C87" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D87" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E87" s="10"/>
+      <c r="F87" s="9"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
@@ -2771,16 +3048,18 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89">
+      <c r="A89" s="9">
         <v>285</v>
       </c>
-      <c r="C89" t="s">
-        <v>231</v>
-      </c>
-      <c r="D89" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="E89" s="9"/>
+      <c r="B89" s="9"/>
+      <c r="C89" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D89" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E89" s="10"/>
+      <c r="F89" s="9"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
@@ -2949,37 +3228,46 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99">
+      <c r="A99" s="9">
         <v>426</v>
       </c>
-      <c r="C99" t="s">
-        <v>231</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100">
+      <c r="A100" s="9">
         <v>449</v>
       </c>
-      <c r="C100" t="s">
-        <v>231</v>
-      </c>
-      <c r="D100" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B100" s="9"/>
+      <c r="C100" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D100" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101">
+      <c r="A101" s="9">
         <v>450</v>
       </c>
-      <c r="C101" t="s">
-        <v>231</v>
-      </c>
-      <c r="D101" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D101" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
@@ -2998,26 +3286,32 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103">
+      <c r="A103" s="9">
         <v>501</v>
       </c>
-      <c r="C103" t="s">
-        <v>231</v>
-      </c>
-      <c r="D103" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D103" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104">
+      <c r="A104" s="9">
         <v>510</v>
       </c>
-      <c r="C104" t="s">
-        <v>231</v>
-      </c>
-      <c r="D104" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B104" s="9"/>
+      <c r="C104" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D104" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
@@ -3036,26 +3330,32 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106">
+      <c r="A106" s="9">
         <v>530</v>
       </c>
-      <c r="C106" t="s">
-        <v>231</v>
-      </c>
-      <c r="D106" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B106" s="9"/>
+      <c r="C106" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D106" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107">
+      <c r="A107" s="9">
         <v>538</v>
       </c>
-      <c r="C107" t="s">
-        <v>231</v>
-      </c>
-      <c r="D107" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B107" s="9"/>
+      <c r="C107" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
@@ -3158,26 +3458,32 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114">
+      <c r="A114" s="9">
         <v>653</v>
       </c>
-      <c r="C114" t="s">
-        <v>231</v>
-      </c>
-      <c r="D114" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B114" s="9"/>
+      <c r="C114" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115">
+      <c r="A115" s="9">
         <v>669</v>
       </c>
-      <c r="C115" t="s">
-        <v>231</v>
-      </c>
-      <c r="D115" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B115" s="9"/>
+      <c r="C115" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D115" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
@@ -3234,37 +3540,46 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119">
+      <c r="A119" s="9">
         <v>700</v>
       </c>
-      <c r="C119" t="s">
-        <v>231</v>
-      </c>
-      <c r="D119" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B119" s="9"/>
+      <c r="C119" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D119" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120">
+      <c r="A120" s="9">
         <v>701</v>
       </c>
-      <c r="C120" t="s">
-        <v>231</v>
-      </c>
-      <c r="D120" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D120" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121">
+      <c r="A121" s="9">
         <v>703</v>
       </c>
-      <c r="C121" t="s">
-        <v>231</v>
-      </c>
-      <c r="D121" s="10" t="s">
-        <v>155</v>
-      </c>
+      <c r="B121" s="9"/>
+      <c r="C121" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
@@ -3341,7 +3656,7 @@
       <c r="C126" t="s">
         <v>231</v>
       </c>
-      <c r="D126" s="10" t="s">
+      <c r="D126" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3352,7 +3667,7 @@
       <c r="C127" t="s">
         <v>231</v>
       </c>
-      <c r="D127" s="10" t="s">
+      <c r="D127" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3445,7 +3760,7 @@
       <c r="C133" t="s">
         <v>231</v>
       </c>
-      <c r="D133" s="10" t="s">
+      <c r="D133" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3474,7 +3789,7 @@
       <c r="C135" t="s">
         <v>231</v>
       </c>
-      <c r="D135" s="10" t="s">
+      <c r="D135" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3503,7 +3818,7 @@
       <c r="C137" t="s">
         <v>231</v>
       </c>
-      <c r="D137" s="10" t="s">
+      <c r="D137" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3582,7 +3897,7 @@
       <c r="C142" t="s">
         <v>231</v>
       </c>
-      <c r="D142" s="10" t="s">
+      <c r="D142" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3625,7 +3940,7 @@
       <c r="C145" t="s">
         <v>231</v>
       </c>
-      <c r="D145" s="10" t="s">
+      <c r="D145" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3668,7 +3983,7 @@
       <c r="C148" t="s">
         <v>231</v>
       </c>
-      <c r="D148" s="10" t="s">
+      <c r="D148" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3727,7 +4042,7 @@
       <c r="C152" t="s">
         <v>231</v>
       </c>
-      <c r="D152" s="10" t="s">
+      <c r="D152" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3802,7 +4117,7 @@
       <c r="C157" t="s">
         <v>231</v>
       </c>
-      <c r="D157" s="10" t="s">
+      <c r="D157" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3829,7 +4144,7 @@
       <c r="C159" t="s">
         <v>231</v>
       </c>
-      <c r="D159" s="10" t="s">
+      <c r="D159" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3872,7 +4187,7 @@
       <c r="C162" t="s">
         <v>231</v>
       </c>
-      <c r="D162" s="10" t="s">
+      <c r="D162" t="s">
         <v>155</v>
       </c>
     </row>
@@ -3915,7 +4230,7 @@
       <c r="C165" t="s">
         <v>231</v>
       </c>
-      <c r="D165" s="10" t="s">
+      <c r="D165" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4022,7 +4337,7 @@
       <c r="C172" t="s">
         <v>231</v>
       </c>
-      <c r="D172" s="10" t="s">
+      <c r="D172" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4033,7 +4348,7 @@
       <c r="C173" t="s">
         <v>231</v>
       </c>
-      <c r="D173" s="10" t="s">
+      <c r="D173" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4236,7 +4551,7 @@
       <c r="C186" t="s">
         <v>231</v>
       </c>
-      <c r="D186" s="10" t="s">
+      <c r="D186" t="s">
         <v>155</v>
       </c>
     </row>
@@ -4514,6 +4829,26 @@
     <hyperlink ref="E91" r:id="rId62" xr:uid="{BCCB328C-B554-403B-BBF3-554A6EC0CDF3}"/>
     <hyperlink ref="E92" r:id="rId63" xr:uid="{567B21AF-B307-4516-A858-4302ED0CF15C}"/>
     <hyperlink ref="E117" r:id="rId64" xr:uid="{E0CCFC97-978E-4E11-9797-4786636AAEF9}"/>
+    <hyperlink ref="E35" r:id="rId65" xr:uid="{1646186D-C865-4762-BDA7-521CB85EF00D}"/>
+    <hyperlink ref="E36" r:id="rId66" xr:uid="{39C8C69A-E143-42CD-8FDD-E59B73D55415}"/>
+    <hyperlink ref="E39" r:id="rId67" xr:uid="{A1A25409-2B65-4D4D-983F-997EDE47EE35}"/>
+    <hyperlink ref="E38" r:id="rId68" xr:uid="{73CA35AE-CA36-45EC-94D8-317DED908269}"/>
+    <hyperlink ref="E46" r:id="rId69" xr:uid="{ACC5C751-142D-4221-8DF5-6DDB9DD385C7}"/>
+    <hyperlink ref="E49" r:id="rId70" xr:uid="{99A53243-7FB9-41E9-A5C8-6F9E3DF3F09C}"/>
+    <hyperlink ref="E50" r:id="rId71" xr:uid="{314A98D8-0996-49C0-83DD-AF25532D7134}"/>
+    <hyperlink ref="E51" r:id="rId72" xr:uid="{8A206375-9124-467C-A2F2-1C155CFAFEBE}"/>
+    <hyperlink ref="E52" r:id="rId73" xr:uid="{302DF96A-B26D-4A92-94A9-3C1750978A54}"/>
+    <hyperlink ref="E53" r:id="rId74" xr:uid="{597C831F-1FC8-43EB-BB15-2A0BB4B8C07E}"/>
+    <hyperlink ref="E54" r:id="rId75" xr:uid="{7EE51D45-B2C1-4554-ABCB-5B9A92CBEDBA}"/>
+    <hyperlink ref="E55" r:id="rId76" xr:uid="{8C2D77A4-727E-4F24-A5E0-249BBE5A8B10}"/>
+    <hyperlink ref="E56" r:id="rId77" xr:uid="{709CAF85-9724-4432-BB4B-D636D00816A6}"/>
+    <hyperlink ref="E3" r:id="rId78" xr:uid="{46DF8277-BAD8-43BC-9961-EB3FDDD5C637}"/>
+    <hyperlink ref="E63" r:id="rId79" xr:uid="{30790F39-F3B0-4BBE-B20F-2DED09102259}"/>
+    <hyperlink ref="E67" r:id="rId80" xr:uid="{BBB70BAB-AF7D-49A9-8D43-1D01CCF9E0FE}"/>
+    <hyperlink ref="E70" r:id="rId81" xr:uid="{48B4B3B2-E7EC-4D4F-9A69-3FC1D5C332BF}"/>
+    <hyperlink ref="E77" r:id="rId82" xr:uid="{56F0EB97-F5AA-4D1B-8CD3-7210D89D0D06}"/>
+    <hyperlink ref="E78" r:id="rId83" xr:uid="{C55A7BE9-513D-443E-A7D7-9CEE888D2015}"/>
+    <hyperlink ref="E34" r:id="rId84" xr:uid="{ADD542F3-6F1E-4EB6-A946-13E8C42F84FF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>